<commit_message>
SMTP Email components and tests
</commit_message>
<xml_diff>
--- a/Data/Config-NadawanieDostepowSAP.xlsx
+++ b/Data/Config-NadawanieDostepowSAP.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa_test02.ADICT\Documents\UiPath\SAP_NadawanieUprawnien\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KatarzynaSmalera\Documents\UiPath\NadawanieDostepowSAP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB0D7BF-8EEF-4552-86BB-7D6AEE15CC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="130">
   <si>
     <t>Name</t>
   </si>
@@ -339,13 +340,107 @@
   </si>
   <si>
     <t>project = FHZ AND summary ~ "TASKTEST*" AND labels not in ("HumanActionRequired") AND description !~ "Zmiana Hierarchii" AND description !~ "SAAMS ID: EXP"</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Email_BodyInitFail</t>
+  </si>
+  <si>
+    <t>Kontatk z RPA team?</t>
+  </si>
+  <si>
+    <t>Email_SubjectInitFail</t>
+  </si>
+  <si>
+    <t>Email_SubjectSE</t>
+  </si>
+  <si>
+    <t>Email_Port</t>
+  </si>
+  <si>
+    <t>Email_Server</t>
+  </si>
+  <si>
+    <t>relay.dlkpl.pl.dalkia.group.ve</t>
+  </si>
+  <si>
+    <t>Email_SenderName</t>
+  </si>
+  <si>
+    <t>RPA</t>
+  </si>
+  <si>
+    <t>Email_SenderAddress</t>
+  </si>
+  <si>
+    <t>rpa@veolia.com</t>
+  </si>
+  <si>
+    <t>Email_RecipmentsSE</t>
+  </si>
+  <si>
+    <t>Email_RecipmentsSuccess</t>
+  </si>
+  <si>
+    <t>Email_RecipmentDevMode</t>
+  </si>
+  <si>
+    <t>Nadawanie Uprawnień SAP - Initialization Fail</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;h4&gt;Dzień dobry,&lt;/h4&gt;
+&lt;p&gt;&lt;strong&gt;Data i czas procesowania:&lt;/strong&gt;&lt;br&gt;&lt;DateTimeNow&gt;&lt;br&gt;RPA-Nadawanie Uprawnień SAP&lt;br&gt;&lt;/p&gt;
+&lt;p&gt;Wystąpił błąd podczas procesowania numeru &lt;strong&gt;NIP:&lt;NIP&gt;&lt;/strong&gt;.&lt;br&gt;
+&lt;strong&gt;Żródło błędu:&lt;/strong&gt;&lt;br&gt;&lt;strExeptionSource&gt;&lt;/p&gt;&lt;p style=""color:red;""&gt;&lt;strong&gt;
+Komunikat o błędzie:&lt;/strong&gt;&lt;br&gt;&lt;strExeptionMessage&gt;&lt;/p&gt;
+&lt;p&gt;W razie potrzeby proszę o kontakt z zespołem RPA.&lt;/p&gt;
+&lt;p&gt;Przepraszam za niedogodności.&lt;br&gt; 
+Wiadomość wygenerowana automatycznie - prosimy nie odpowiadać na podany adres e-mail.&lt;/p&gt;
+&lt;p&gt;Miłego dnia! &lt;br&gt; 
+Robot&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Nadawanie Uprawnień SAP - System Exception</t>
+  </si>
+  <si>
+    <t>katarzyna.widlo@office-samurai.com</t>
+  </si>
+  <si>
+    <t>Development_Mode</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;h4&gt;Dzień dobry,&lt;/h4&gt;
+&lt;p&gt;&lt;strong&gt;Data i czas procesowania:&lt;/strong&gt;&lt;br&gt;&lt;DateTimeNow&gt;&lt;/p&gt;RPA-Nadawanie Uprawnień SAP&lt;br&gt;&lt;br&gt;&lt;p&gt;Wystąpił błąd podczas inicjalizacji procesu.&lt;br&gt;Robot nie rozpoczął procesowania z powodu błędu.&lt;br&gt;Żadne zadanie Jira nie zostało zweryfikowane.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Żródło błędu:&lt;/strong&gt;&lt;br&gt;&lt;strExeptionSource&gt;&lt;/p&gt;&lt;p style=""color:red;""&gt;&lt;strong&gt;Komunikat o błędzie:&lt;/strong&gt;&lt;br&gt;&lt;strExeptionMessage&gt;&lt;/p&gt;&lt;p&gt;Prosze zrestartować robota ręcznie.&lt;br&gt;W razie potrzeby proszę o kontakt z zespołem RPA.&lt;/p&gt;&lt;br&gt;&lt;p&gt;Przepraszam za niedogodności.&lt;br&gt; Wiadomość wygenerowana automatycznie - prosimy nie odpowiadać na podany adres e-mail.&lt;/p&gt;&lt;p&gt;Miłego dnia! &lt;br&gt; Robot&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Email_BodyDispatcherSE</t>
+  </si>
+  <si>
+    <t>Email_BodyPerformerSE</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;&lt;h4&gt;Dzień dobry,&lt;/h4&gt;
+&lt;p&gt;&lt;strong&gt;Data i czas procesowania:&lt;/strong&gt;&lt;br&gt;&lt;DateTimeNow&gt;&lt;br&gt;RPA-Nadawanie Uprawnień SAP&lt;br&gt;&lt;/p&gt;
+&lt;p&gt;Wystąpił błąd podczas pobierania zadań z Jira.
+&lt;strong&gt;Żródło błędu:&lt;/strong&gt;&lt;br&gt;&lt;strExeptionSource&gt;&lt;/p&gt;&lt;p style=""color:red;""&gt;&lt;strong&gt;
+Komunikat o błędzie:&lt;/strong&gt;&lt;br&gt;&lt;strExeptionMessage&gt;&lt;/p&gt;
+&lt;p&gt;W razie potrzeby proszę o kontakt z zespołem RPA.&lt;/p&gt;
+&lt;p&gt;Przepraszamy za niedogodności.&lt;br&gt; 
+Wiadomość wygenerowana automatycznie - prosimy nie odpowiadać na podany adres e-mail.&lt;/p&gt;
+&lt;p&gt;Miłego dnia! &lt;br&gt; 
+Robot&lt;/p&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>wanda.kurowska@office-samurai.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -398,8 +493,15 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +520,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -432,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -457,13 +571,31 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -774,11 +906,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA989"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -900,277 +1032,392 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:27">
+      <c r="C7" s="2"/>
+      <c r="D7" s="4"/>
+    </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1">
+      <c r="A10" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
+    <row r="12" spans="1:27" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15" customHeight="1">
-      <c r="A12" t="s">
+    <row r="14" spans="1:27" ht="15" customHeight="1">
+      <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15" customHeight="1">
-      <c r="A13" t="s">
+    <row r="15" spans="1:27" ht="15" customHeight="1">
+      <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" s="10" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A22" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" s="10" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A23" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="9"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
     </row>
     <row r="24" spans="1:4" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" s="10" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A25" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" s="10" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>89</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A31" s="14" t="s">
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A33" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="150">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>80</v>
+        <v>69</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1">
       <c r="A36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="150">
+      <c r="A37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A38" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="8" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A37" s="8" t="s">
+    <row r="39" spans="1:4" s="8" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A39" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A38" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A39" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A40" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A41" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A42" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C42" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A45" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="16"/>
+    </row>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A54" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -2096,11 +2343,14 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A33:D33"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2109,7 +2359,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3321,11 +3571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>